<commit_message>
files and results updated
</commit_message>
<xml_diff>
--- a/datos_relu.xlsx
+++ b/datos_relu.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -785,6 +785,42 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>3</v>
+      </c>
+      <c r="B11" t="n">
+        <v>50</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.005889368057250976</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1111.130075874329</v>
+      </c>
+      <c r="E11" t="n">
+        <v>1200.114905548096</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>75.69570599999999</v>
+      </c>
+      <c r="H11" t="n">
+        <v>135.962256</v>
+      </c>
+      <c r="I11" t="n">
+        <v>489.28846</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>